<commit_message>
initial push for new branch
</commit_message>
<xml_diff>
--- a/cypress/e2e/Reports/BalanceChecker/Topup_Balance.xlsx
+++ b/cypress/e2e/Reports/BalanceChecker/Topup_Balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workplace\PAYSTAGE-AUTOMATION\cypress\e2e\Reports\BalanceChecker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2098A540-3430-4702-8F3B-2EA70373FFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7BAB2D-EA86-48E5-9268-A0B7B7C6914E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,7 +432,7 @@
   <dimension ref="A1:J965"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>